<commit_message>
Fix brain investment literal eval + venv
</commit_message>
<xml_diff>
--- a/parameters/tickers_names.xlsx
+++ b/parameters/tickers_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1956\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC8AF80A-697C-442B-A2C5-5EB8BCA0E7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{EF5806C6-8A8A-4437-8647-120280FF41A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3DD1700-307C-4D86-83F8-E117B4B0301C}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4596,7 +4596,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4727,6 +4727,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5073,8 +5080,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5430,10 +5438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E531"/>
+  <dimension ref="A1:F531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -5441,7 +5449,7 @@
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5458,7 +5466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5475,7 +5483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5492,7 +5500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -5508,8 +5516,9 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -5526,7 +5535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5543,7 +5552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -5560,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5577,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -5594,7 +5603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -5611,7 +5620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -5628,7 +5637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -5645,7 +5654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -5662,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -5679,7 +5688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -5696,7 +5705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>47</v>
       </c>

</xml_diff>